<commit_message>
Update SensorBox_Component_Tracker.xlsx added the box numbers
</commit_message>
<xml_diff>
--- a/Sensor Box Deployment Inventory /SensorBox_Component_Tracker.xlsx
+++ b/Sensor Box Deployment Inventory /SensorBox_Component_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allensong/Documents/GitHub/CommonSENSES/Sensor Box Inventory /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriishhate/GitHub/CommonSENSES/Sensor Box Deployment Inventory /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E31DE3-2970-524B-B93B-8061DD03DD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C00D8A8-51E6-9A49-A93F-7B738A546C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="1840" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
+    <workbookView xWindow="6920" yWindow="1840" windowWidth="27640" windowHeight="16940" xr2:uid="{9F8D9832-C5EF-1142-B4F9-7517213DD771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="116">
   <si>
     <t>Box Number</t>
   </si>
@@ -775,7 +775,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,6 +804,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -818,6 +821,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -832,6 +838,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -846,6 +855,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -860,6 +872,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -874,6 +889,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -888,6 +906,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -902,6 +923,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -916,6 +940,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -930,6 +957,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -944,6 +974,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -958,6 +991,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -972,6 +1008,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -986,6 +1025,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -1000,6 +1042,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1013,7 +1058,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1075,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -1041,7 +1092,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +1109,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1126,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1143,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -1097,7 +1160,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -1111,7 +1177,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
@@ -1125,7 +1194,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="B25" t="s">
         <v>29</v>
       </c>
@@ -1139,7 +1211,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="B26" t="s">
         <v>30</v>
       </c>
@@ -1153,7 +1228,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
@@ -1167,7 +1245,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -1181,7 +1262,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="B29" t="s">
         <v>33</v>
       </c>
@@ -1195,7 +1279,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="B30" t="s">
         <v>34</v>
       </c>
@@ -1209,7 +1296,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
@@ -1223,7 +1313,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="B32" t="s">
         <v>36</v>
       </c>
@@ -1237,7 +1330,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
@@ -1251,7 +1347,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="B34" t="s">
         <v>38</v>
       </c>
@@ -1265,7 +1364,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B35" t="s">
         <v>39</v>
       </c>
@@ -1279,7 +1381,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B36" t="s">
         <v>40</v>
       </c>
@@ -1293,7 +1398,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="B37" t="s">
         <v>41</v>
       </c>
@@ -1307,7 +1415,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="B38" t="s">
         <v>42</v>
       </c>
@@ -1321,7 +1432,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="B39" t="s">
         <v>43</v>
       </c>
@@ -1335,7 +1449,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="B40" t="s">
         <v>44</v>
       </c>
@@ -1349,7 +1466,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="B41" t="s">
         <v>45</v>
       </c>
@@ -1363,7 +1483,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="B42" t="s">
         <v>46</v>
       </c>
@@ -1377,7 +1500,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="B43" t="s">
         <v>47</v>
       </c>
@@ -1391,7 +1517,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="B44" t="s">
         <v>48</v>
       </c>
@@ -1405,7 +1534,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="B45" t="s">
         <v>49</v>
       </c>
@@ -1419,7 +1551,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -1433,7 +1568,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B47" t="s">
         <v>51</v>
       </c>
@@ -1447,7 +1585,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -1461,7 +1602,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="B49" t="s">
         <v>53</v>
       </c>
@@ -1475,7 +1619,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="B50" t="s">
         <v>54</v>
       </c>
@@ -1489,7 +1636,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="B51" t="s">
         <v>55</v>
       </c>
@@ -1503,7 +1653,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B52" t="s">
         <v>56</v>
       </c>
@@ -1517,7 +1670,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="B53" t="s">
         <v>57</v>
       </c>
@@ -1531,7 +1687,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="B54" t="s">
         <v>58</v>
       </c>
@@ -1545,7 +1704,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="B55" t="s">
         <v>59</v>
       </c>
@@ -1559,7 +1721,10 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="B56" t="s">
         <v>60</v>
       </c>

</xml_diff>